<commit_message>
change Huy's work, add file report
</commit_message>
<xml_diff>
--- a/WorkTable.xlsx
+++ b/WorkTable.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lai Minh Thong\Documents\GitHub\Synthesis-Report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\UNIVERSITY\DataStructure\Synthesis-Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60456BB-5D8D-4214-AFDD-6AF1D0E6B2D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7F32BF-34E0-43EE-8E65-26BCA21CD1F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2985" yWindow="2880" windowWidth="21600" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28785" yWindow="2085" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Huy</t>
   </si>
@@ -45,9 +45,6 @@
     <t>AVL, BST, Red Black</t>
   </si>
   <si>
-    <t>Hashtable</t>
-  </si>
-  <si>
     <t>B-tree, Multi-tree</t>
   </si>
   <si>
@@ -84,10 +81,10 @@
     <t>Jump Search</t>
   </si>
   <si>
-    <t>Post sort</t>
-  </si>
-  <si>
-    <t>HIHIHIHIH</t>
+    <t>HashMap</t>
+  </si>
+  <si>
+    <t>Hashtable, ADT, Analysis of Algorithms</t>
   </si>
 </sst>
 </file>
@@ -471,73 +468,71 @@
   <dimension ref="B2:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="3" max="3" width="25.88671875" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="35.28515625" customWidth="1"/>
-    <col min="6" max="7" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="35.33203125" customWidth="1"/>
+    <col min="6" max="7" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="10.15" customHeight="1"/>
+    <row r="2" spans="2:6" ht="10.199999999999999" customHeight="1"/>
     <row r="3" spans="2:6" hidden="1"/>
-    <row r="4" spans="2:6" ht="32.450000000000003" customHeight="1">
+    <row r="4" spans="2:6" ht="32.4" customHeight="1">
       <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>10</v>
-      </c>
       <c r="E4" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="29.45" customHeight="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="29.4" customHeight="1">
       <c r="B5" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>20</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="F5" s="1"/>
     </row>
     <row r="6" spans="2:6" ht="27.6" customHeight="1">
       <c r="B6" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="28.15" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="28.2" customHeight="1">
       <c r="B7" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="29.45" customHeight="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="29.4" customHeight="1">
       <c r="B8" s="5" t="s">
         <v>3</v>
       </c>
@@ -546,7 +541,7 @@
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="30" customHeight="1">
@@ -554,16 +549,16 @@
         <v>4</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="2:6">
       <c r="B11" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>

</xml_diff>

<commit_message>
merge Huy, Thong files
</commit_message>
<xml_diff>
--- a/WorkTable.xlsx
+++ b/WorkTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\UNIVERSITY\DataStructure\Synthesis-Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7F32BF-34E0-43EE-8E65-26BCA21CD1F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA1AEA1C-D7A1-4761-BA45-B3958C786B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28785" yWindow="2085" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3324" yWindow="1872" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -81,10 +81,10 @@
     <t>Jump Search</t>
   </si>
   <si>
-    <t>HashMap</t>
-  </si>
-  <si>
     <t>Hashtable, ADT, Analysis of Algorithms</t>
+  </si>
+  <si>
+    <t>Trie tree</t>
   </si>
 </sst>
 </file>
@@ -467,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -498,13 +498,13 @@
         <v>0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F5" s="1"/>
     </row>

</xml_diff>